<commit_message>
added new Testcase for OneWayBooking Full
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="OneWayBooking" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,20 +21,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
   <si>
     <t xml:space="preserve">agileway</t>
   </si>
   <si>
     <t xml:space="preserve">testwise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oneway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joseph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lieven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">master</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hamilton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobbson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wilson</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -101,12 +133,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -301,7 +341,7 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -324,4 +364,156 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="25.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="n">
+        <v>4659908765341267</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>4659908765341267</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>4659908765341267</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>4659908765341267</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>4659908765341267</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2" type="custom">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G1" type="textLength">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>